<commit_message>
max block adj partially implemented
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
+++ b/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
@@ -5,20 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Primary Location" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Max Block Adjacency" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Base Measure" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Block Percent" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Anchor" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Max Block Composition" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Block Orientation" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Blocking" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Product Sequence" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Result" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Max Block Adjacency SubCat" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Base Measure" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Block Percent" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Anchor" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Max Block Composition" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Block Orientation" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Blocking" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Product Sequence" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Result" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$H$39</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="172">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -183,6 +184,9 @@
     <t xml:space="preserve">Fruit MSL </t>
   </si>
   <si>
+    <t xml:space="preserve">Fruit MSL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Are the majority of Nat/Org Grain SKUs blocked together?</t>
   </si>
   <si>
@@ -201,6 +205,9 @@
     <t xml:space="preserve">In an Integrated Bars set, when grain segments are vertically blocked, what Grain Segment is Adjacent to Nutrition?</t>
   </si>
   <si>
+    <t xml:space="preserve">Max Block Adjacency SubCat</t>
+  </si>
+  <si>
     <t xml:space="preserve">What is the Base Footage of Grain Bars in Grain MSL?</t>
   </si>
   <si>
@@ -216,9 +223,6 @@
     <t xml:space="preserve">What is the base footage of Fruit Snacks in the Fruit Snacks MSL?</t>
   </si>
   <si>
-    <t xml:space="preserve">Fruit MSL</t>
-  </si>
-  <si>
     <t xml:space="preserve">What is the base footage of Total Bars in an Integrated Bars set?</t>
   </si>
   <si>
@@ -259,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve">Scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short Name</t>
   </si>
   <si>
     <t xml:space="preserve">Result</t>
@@ -324,31 +331,40 @@
     <t xml:space="preserve">B Param 1</t>
   </si>
   <si>
+    <t xml:space="preserve">B Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Required Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Required Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Required Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Required Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUTRITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nature Valley </t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxadjc</t>
+  </si>
+  <si>
     <t xml:space="preserve">B Value 2</t>
   </si>
   <si>
-    <t xml:space="preserve">A Required Param 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">A Required Value</t>
   </si>
   <si>
-    <t xml:space="preserve">B Required Param 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">B Required Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUTRITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nature Valley </t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxadjc</t>
   </si>
   <si>
     <t xml:space="preserve">maxadjc1</t>
@@ -547,7 +563,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -575,6 +591,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -660,7 +682,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -697,15 +719,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -713,11 +735,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -848,19 +874,19 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.3036437246964"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3846153846154"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.2348178137652"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1417,7 +1443,7 @@
         <v>48</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>10</v>
@@ -1428,7 +1454,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>30</v>
@@ -1446,7 +1472,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>19</v>
@@ -1464,17 +1490,17 @@
     </row>
     <row r="28" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>17</v>
@@ -1488,10 +1514,10 @@
     </row>
     <row r="29" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
@@ -1512,10 +1538,10 @@
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1532,16 +1558,16 @@
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>10</v>
@@ -1552,16 +1578,16 @@
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>10</v>
@@ -1572,10 +1598,10 @@
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
@@ -1596,10 +1622,10 @@
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
@@ -1620,10 +1646,10 @@
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
@@ -1644,10 +1670,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
@@ -1668,10 +1694,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
@@ -1692,10 +1718,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1705,15 +1731,15 @@
         <v>10</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1723,7 +1749,7 @@
         <v>10</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1762,47 +1788,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.165991902834"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.4858299595142"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>73</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>138</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1821,280 +1912,339 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="133.789473684211"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="134.971659919028"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" s="12" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="B17" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>144</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>165</v>
+      <c r="A18" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" s="12" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>144</v>
+    <row r="19" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>149</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
@@ -2116,45 +2266,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.3765182186235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.0607287449393"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.9109311740891"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2162,117 +2315,131 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="9"/>
+      <c r="H6" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>90</v>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2291,110 +2458,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.7732793522267"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.3076923076923"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="12.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
         <v>104</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2413,19 +2563,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:J65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.5546558704453"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.3076923076923"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,127 +2586,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
+        <v>88</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2570,18 +2654,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.9797570850202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.3036437246964"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2590,103 +2674,125 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>112</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>109</v>
+    </row>
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2705,71 +2811,123 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.7327935222672"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="63.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>67</v>
+      <c r="D4" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2788,93 +2946,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="12" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="63.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>124</v>
+      <c r="E3" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2893,19 +3029,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.165991902834"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2913,78 +3051,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>127</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3004,20 +3134,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.8421052631579"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3025,91 +3154,79 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>115</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>131</v>
+      <c r="C6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
max block composition exists in max block blocking
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
+++ b/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,13 +16,15 @@
     <sheet name="Block Percent" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Anchor" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Max Block Composition" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Block Orientation" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Blocking" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Product Sequence" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Result" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Exists in Max Block" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Block Orientation" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Blocking" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Product Sequence" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Result" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$H$39</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$B$1:$B$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$I$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="182">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -54,6 +56,9 @@
     <t xml:space="preserve">Found Scene</t>
   </si>
   <si>
+    <t xml:space="preserve">Run on Empty SCIF</t>
+  </si>
+  <si>
     <t xml:space="preserve">store_type</t>
   </si>
   <si>
@@ -99,7 +104,7 @@
     <t xml:space="preserve">When there is a Non-Integrated Bars set, what Nutrition segments are present in the Nutrition MSL?</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-Integrated Bars Set Present</t>
+    <t xml:space="preserve">!Non-Integrated Bars Set Present</t>
   </si>
   <si>
     <t xml:space="preserve">Nutrition MSL</t>
@@ -154,6 +159,9 @@
     <t xml:space="preserve">In a Non-Integrated set, are Nutrition Bars Blocked Vertically  in the Nutrition MSL?</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-Integrated Bars Set Present</t>
+  </si>
+  <si>
     <t xml:space="preserve">In a Non-Integrated set, are Nutrition Wellness Bars Blocked Vertically  in the Nutrition MSL?</t>
   </si>
   <si>
@@ -191,6 +199,9 @@
   </si>
   <si>
     <t xml:space="preserve">Are Annie's Grain items stocked with Kids Grain?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exists in Max Block</t>
   </si>
   <si>
     <t xml:space="preserve">In the Grain MSL when grain segments are vertically blocked, what is the Flow of the Grain Snack Segments (Left to Right)?</t>
@@ -412,22 +423,40 @@
     <t xml:space="preserve">LEFT </t>
   </si>
   <si>
+    <t xml:space="preserve">Segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail Result</t>
+  </si>
+  <si>
     <t xml:space="preserve">GRAIN, NUTRITION, FRUIT, TOASTER PASTRIES</t>
   </si>
   <si>
+    <t xml:space="preserve">Could not determine</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maxblock</t>
   </si>
   <si>
     <t xml:space="preserve">MaxblockC</t>
   </si>
   <si>
-    <t xml:space="preserve">Brand</t>
+    <t xml:space="preserve">Numerator Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator Value 1</t>
   </si>
   <si>
     <t xml:space="preserve">ANNIE'S HOMEGROWN</t>
   </si>
   <si>
-    <t xml:space="preserve">GRAIN KIDS</t>
+    <t xml:space="preserve">GRAIN KID</t>
   </si>
   <si>
     <t xml:space="preserve">MaxblockC1</t>
@@ -448,9 +477,6 @@
     <t xml:space="preserve">BlkOrientation1</t>
   </si>
   <si>
-    <t xml:space="preserve">BRAND</t>
-  </si>
-  <si>
     <t xml:space="preserve">blk</t>
   </si>
   <si>
@@ -460,6 +486,9 @@
     <t xml:space="preserve">PRIVATE LABEL</t>
   </si>
   <si>
+    <t xml:space="preserve">Not Present in Grain MSL</t>
+  </si>
+  <si>
     <t xml:space="preserve">blk1</t>
   </si>
   <si>
@@ -529,7 +558,7 @@
     <t xml:space="preserve">; </t>
   </si>
   <si>
-    <t xml:space="preserve">Nutrition, TP, Fruit; Nutrition, Fruit; Nutrition, TP; TP, Fruit; Nutrition; Fruit; TP; Only Grain; Could not determine</t>
+    <t xml:space="preserve">Nutrition, Toaster Pastries, Fruit; Nutrition, Fruit; Nutrition, Toaster Pastries; Toaster Pastries, Fruit; Nutrition; Fruit; Toaster Pastries; Only Grain; Could not determine</t>
   </si>
   <si>
     <t xml:space="preserve">Performance, Wellness, Diet; Performance, Wellness; Performance, Diet;  Wellness, Diet; Performance; Wellness; Diet; Could not determine</t>
@@ -566,7 +595,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -596,18 +625,23 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -685,7 +719,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -722,31 +756,35 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -869,31 +907,35 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.8785425101215"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -918,862 +960,912 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="20" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="6"/>
       <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="D13" s="4"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="E16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I22" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="D23" s="4"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I23" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="20.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I24" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="17" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I26" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I28" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G30" s="3"/>
       <c r="H30" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I30" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G34" s="3"/>
       <c r="H34" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I34" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G36" s="3"/>
       <c r="H36" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G37" s="3"/>
       <c r="H37" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="G38" s="3"/>
       <c r="H38" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="G39" s="3"/>
       <c r="H39" s="3" t="s">
-        <v>69</v>
+        <v>11</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B39">
+    <filterColumn colId="0">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Blocking"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="C28">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$U28="Ready"</formula>
+      <formula>$V28="Ready"</formula>
     </cfRule>
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$U28="Removed"</formula>
+      <formula>$V28="Removed"</formula>
     </cfRule>
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$U28="Done"</formula>
+      <formula>$V28="Done"</formula>
     </cfRule>
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$U28="Built"</formula>
+      <formula>$V28="Built"</formula>
     </cfRule>
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>$U28="Templated"</formula>
+      <formula>$V28="Templated"</formula>
     </cfRule>
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>$U28&lt;&gt;""</formula>
+      <formula>$V28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1783,6 +1875,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1791,20 +1884,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.4858299595142"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,91 +1904,79 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>137</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>89</v>
+        <v>120</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>120</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>137</v>
+      <c r="C6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1915,47 +1995,123 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.0202429149798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>144</v>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1974,283 +2130,342 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="134.971659919028"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="136.255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+    <row r="1" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="B16" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B17" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" s="13" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>150</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2271,19 +2486,19 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.9109311740891"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4898785425101"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.4493927125506"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2292,157 +2507,157 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2469,16 +2684,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.8421052631579"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.8825910931174"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2487,81 +2702,81 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>0.25</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2583,18 +2798,18 @@
   <dimension ref="A1:J65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.8421052631579"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2603,55 +2818,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2679,10 +2894,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.3036437246964"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2691,125 +2906,125 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>113</v>
+        <v>91</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2836,9 +3051,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.7327935222672"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="85.4817813765182"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2848,103 +3063,103 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2971,63 +3186,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.6315789473684"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+    <row r="1" s="11" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>77</v>
+      <c r="B1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="63.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3046,93 +3261,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.8825910931174"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="F2" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="F3" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3151,99 +3352,61 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1821862348178"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1578947368421"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7732793522267"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>135</v>
+        <v>120</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
base measure block orientation block percent dependency updates catchall bug fix
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
+++ b/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,18 +13,19 @@
     <sheet name="Max Block Adjacency" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Max Block Adjacency SubCat" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Base Measure" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Block Percent" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Anchor" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Max Block Composition" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Exists in Max Block" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Anchor" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Max Block Composition" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Exists in Max Block" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Block Percent" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Block Orientation" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Blocking" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Product Sequence" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Result" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$B$1:$B$39</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$I$39</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$I$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$B$1:$B$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$I$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="186">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -104,7 +105,7 @@
     <t xml:space="preserve">When there is a Non-Integrated Bars set, what Nutrition segments are present in the Nutrition MSL?</t>
   </si>
   <si>
-    <t xml:space="preserve">!Non-Integrated Bars Set Present</t>
+    <t xml:space="preserve">Non-Integrated Bars Set Present</t>
   </si>
   <si>
     <t xml:space="preserve">Nutrition MSL</t>
@@ -116,12 +117,18 @@
     <t xml:space="preserve">Block Orientation</t>
   </si>
   <si>
-    <t xml:space="preserve">Not Blocked</t>
+    <t xml:space="preserve">Are All Family Grain Snacks Blocked Vertically  in the Grain MSL?, Are Adult Grain Snacks Blocked Vertically  in the Grain MSL?, Are Kid Grain Snacks Blocked Vertically  in the Grain MSL?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,,</t>
   </si>
   <si>
     <t xml:space="preserve">Are All Family Grain Snacks Blocked Vertically  in the Grain MSL?</t>
   </si>
   <si>
+    <t xml:space="preserve">Block Percent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Are Adult Grain Snacks Blocked Vertically  in the Grain MSL?</t>
   </si>
   <si>
@@ -137,19 +144,15 @@
     <t xml:space="preserve">In an Integrated Bars Set, are Nutrition Bars Blocked Vertically  in the Grain MSL?</t>
   </si>
   <si>
-    <t xml:space="preserve">Block Percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrated Bars Set Present,
-Not Blocked</t>
+    <t xml:space="preserve">What % of stores have an Integrated Bars set in the Grain MSL?; In an Integrated Bars Set, are Nutrition Wellness Bars Blocked Vertically  in the Grain MSL?; In an Integrated Bars Set, are Nutrition Performance Bars Blocked Vertically  in Grain MSL?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated Bars Set Present,,</t>
   </si>
   <si>
     <t xml:space="preserve">In an Integrated Bars Set, are Nutrition Wellness Bars Blocked Vertically  in the Grain MSL?</t>
   </si>
   <si>
-    <t xml:space="preserve">What % of stores have an Integrated Bars set in the Grain MSL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Integrated Bars Set Present</t>
   </si>
   <si>
@@ -159,7 +162,10 @@
     <t xml:space="preserve">In a Non-Integrated set, are Nutrition Bars Blocked Vertically  in the Nutrition MSL?</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-Integrated Bars Set Present</t>
+    <t xml:space="preserve">What % of stores have an Integrated Bars set in the Grain MSL?; In a Non-Integrated set, are Nutrition Wellness Bars Blocked Vertically  in the Nutrition MSL?; In a Non-Integrated set, are Nutrition Performance Bars Blocked Vertically  in Nutrition MSL?; In a Non-Integrated set, are Nutrition Diet Bars Blocked Vertically  in the Nutrition MSL?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Integrated Bars Set Present,,,</t>
   </si>
   <si>
     <t xml:space="preserve">In a Non-Integrated set, are Nutrition Wellness Bars Blocked Vertically  in the Nutrition MSL?</t>
@@ -387,6 +393,12 @@
     <t xml:space="preserve">maxadjc1</t>
   </si>
   <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max</t>
+  </si>
+  <si>
     <t xml:space="preserve">shelf length</t>
   </si>
   <si>
@@ -399,81 +411,84 @@
     <t xml:space="preserve">GRAIN,NUTRITION</t>
   </si>
   <si>
+    <t xml:space="preserve"> GRAIN, NUTRITION, FRUIT, TOASTER PASTRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIGHT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEFT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN, NUTRITION, FRUIT, TOASTER PASTRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could not determine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxblock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATED SUBCATEGORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxblockC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANNIE'S HOMEGROWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN KID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxblockC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTRN WELLNESS</t>
+  </si>
+  <si>
     <t xml:space="preserve">BlkPercent </t>
   </si>
   <si>
-    <t xml:space="preserve">UPDATED SUBCATEGORY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTRN WELLNESS</t>
-  </si>
-  <si>
     <t xml:space="preserve">NTRN PERFORMANCE</t>
   </si>
   <si>
     <t xml:space="preserve">NTRN DIET</t>
   </si>
   <si>
-    <t xml:space="preserve"> GRAIN, NUTRITION, FRUIT, TOASTER PASTRIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIGHT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEFT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN, NUTRITION, FRUIT, TOASTER PASTRIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Could not determine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxblock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxblockC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerator Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerator Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANNIE'S HOMEGROWN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN KID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxblockC1</t>
+    <t xml:space="preserve">GRAIN ALL FAMILY </t>
   </si>
   <si>
     <t xml:space="preserve">BlkOrientation</t>
   </si>
   <si>
-    <t xml:space="preserve">GRAIN ALL FAMILY </t>
-  </si>
-  <si>
     <t xml:space="preserve">GRAIN ADULT </t>
   </si>
   <si>
     <t xml:space="preserve">GRAIN KIDS </t>
   </si>
   <si>
+    <t xml:space="preserve">Not Present in Grain MSL</t>
+  </si>
+  <si>
     <t xml:space="preserve">BlkOrientation1</t>
   </si>
   <si>
@@ -484,9 +499,6 @@
   </si>
   <si>
     <t xml:space="preserve">PRIVATE LABEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Present in Grain MSL</t>
   </si>
   <si>
     <t xml:space="preserve">blk1</t>
@@ -619,6 +631,12 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -635,12 +653,6 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -719,7 +731,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,7 +756,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -752,7 +764,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -760,20 +772,24 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -918,20 +934,20 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="86.4453441295547"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.1619433198381"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1111,7 +1127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="20" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -1119,9 +1135,11 @@
         <v>25</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
@@ -1136,10 +1154,10 @@
     </row>
     <row r="10" customFormat="false" ht="17.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>24</v>
@@ -1157,12 +1175,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="41.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
@@ -1180,12 +1198,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>24</v>
@@ -1203,12 +1221,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
@@ -1224,19 +1242,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="7" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>18</v>
@@ -1251,19 +1269,19 @@
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>18</v>
@@ -1276,21 +1294,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>18</v>
@@ -1303,19 +1321,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>18</v>
@@ -1328,21 +1346,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>23</v>
@@ -1355,21 +1373,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>23</v>
@@ -1382,21 +1400,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>23</v>
@@ -1409,12 +1427,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1430,12 +1448,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
@@ -1453,12 +1471,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
@@ -1478,10 +1496,10 @@
     </row>
     <row r="24" customFormat="false" ht="20.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4" t="s">
@@ -1503,20 +1521,20 @@
     </row>
     <row r="25" customFormat="false" ht="17" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
@@ -1526,12 +1544,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
@@ -1547,10 +1565,10 @@
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1566,17 +1584,17 @@
     </row>
     <row r="28" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>18</v>
@@ -1591,17 +1609,17 @@
     </row>
     <row r="29" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>18</v>
@@ -1616,10 +1634,10 @@
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1637,16 +1655,16 @@
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
@@ -1658,16 +1676,16 @@
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
@@ -1679,17 +1697,17 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>18</v>
@@ -1704,17 +1722,17 @@
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>18</v>
@@ -1729,17 +1747,17 @@
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>18</v>
@@ -1754,17 +1772,17 @@
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>18</v>
@@ -1779,17 +1797,17 @@
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>23</v>
@@ -1804,10 +1822,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1818,15 +1836,15 @@
         <v>11</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1837,35 +1855,35 @@
         <v>11</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B39">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:I39">
+    <filterColumn colId="1">
       <customFilters and="true">
-        <customFilter operator="equal" val="Blocking"/>
+        <customFilter operator="equal" val="Block Orientation"/>
       </customFilters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="C28">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$V28="Ready"</formula>
+      <formula>KPIs!$V28="Ready"</formula>
     </cfRule>
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$V28="Removed"</formula>
+      <formula>KPIs!$V28="Removed"</formula>
     </cfRule>
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$V28="Done"</formula>
+      <formula>KPIs!$V28="Done"</formula>
     </cfRule>
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$V28="Built"</formula>
+      <formula>KPIs!$V28="Built"</formula>
     </cfRule>
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>$V28="Templated"</formula>
+      <formula>KPIs!$V28="Templated"</formula>
     </cfRule>
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>$V28&lt;&gt;""</formula>
+      <formula>KPIs!$V28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1884,17 +1902,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -1904,81 +1922,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1997,18 +1985,18 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.0202429149798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2017,49 +2005,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -2067,51 +2055,51 @@
         <v>148</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>148</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2138,9 +2126,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -2150,27 +2138,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2192,277 +2180,277 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="136.255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="137.433198380567"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>157</v>
+    <row r="1" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>158</v>
+      <c r="A2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>160</v>
+      <c r="A3" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>161</v>
+      <c r="A4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>162</v>
+      <c r="A5" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>159</v>
-      </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>159</v>
+    <row r="7" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>167</v>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>171</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>169</v>
+      <c r="A9" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>170</v>
+      <c r="A10" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="14" t="s">
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>171</v>
-      </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" s="14" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>159</v>
+    <row r="19" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
@@ -2492,13 +2480,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2507,25 +2495,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2533,21 +2521,21 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2555,21 +2543,21 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2577,21 +2565,21 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,65 +2587,65 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2684,16 +2672,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.8421052631579"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.4858299595142"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2702,40 +2690,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2743,40 +2731,40 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>0.25</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2803,13 +2791,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.8421052631579"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.4858299595142"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2818,55 +2806,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2886,145 +2874,201 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5101214574899"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>122</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3043,123 +3087,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="85.4817813765182"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="11" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="63.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>121</v>
+        <v>93</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3178,71 +3170,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="63.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>70</v>
+      <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>124</v>
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>93</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>124</v>
+        <v>93</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>71</v>
+        <v>131</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3261,18 +3261,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3281,59 +3283,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3352,21 +3334,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1821862348178"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1578947368421"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7732793522267"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.2307692307692"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3374,39 +3354,153 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>53</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>120</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stocked location max block adjacency sub
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
+++ b/Projects/GMIUS/Data/Snacks GMI KPI Template v0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,12 +20,13 @@
     <sheet name="Block Orientation" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Blocking" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Product Sequence" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Result" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Stocked Location" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Result" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$I$39</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$J$39</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$B$1:$B$39</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$I$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$J$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="193">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -57,6 +58,9 @@
     <t xml:space="preserve">Found Scene</t>
   </si>
   <si>
+    <t xml:space="preserve">Dependency Fail Result</t>
+  </si>
+  <si>
     <t xml:space="preserve">Run on Empty SCIF</t>
   </si>
   <si>
@@ -195,9 +199,6 @@
     <t xml:space="preserve">Where are the majority of Nat/Org Fruit Snacks stocked?</t>
   </si>
   <si>
-    <t xml:space="preserve">Fruit MSL </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fruit MSL</t>
   </si>
   <si>
@@ -210,7 +211,7 @@
     <t xml:space="preserve">Exists in Max Block</t>
   </si>
   <si>
-    <t xml:space="preserve">In the Grain MSL when grain segments are vertically blocked, what is the Flow of the Grain Snack Segments (Left to Right)?</t>
+    <t xml:space="preserve">In the Grain MSL when grain segs are vertically blkd, what is the Flow of the Grain Snack seg (L&gt;R)?</t>
   </si>
   <si>
     <t xml:space="preserve">Product Sequence</t>
@@ -219,12 +220,15 @@
     <t xml:space="preserve">Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve">In an Integrated Bars set, when grain segments are vertically blocked, what Grain Segment is Adjacent to Nutrition?</t>
+    <t xml:space="preserve">In an Integrated Bars set, when grain segments are vertically blkd, what Grain Seg is Adj to Ntrn?</t>
   </si>
   <si>
     <t xml:space="preserve">Max Block Adjacency SubCat</t>
   </si>
   <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
     <t xml:space="preserve">What is the Base Footage of Grain Bars in Grain MSL?</t>
   </si>
   <si>
@@ -271,12 +275,6 @@
   </si>
   <si>
     <t xml:space="preserve">Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Param 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value 2</t>
   </si>
   <si>
     <t xml:space="preserve">Scene_type</t>
@@ -321,196 +319,223 @@
     <t xml:space="preserve">PrimaryLocationN </t>
   </si>
   <si>
+    <t xml:space="preserve">A Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Required Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Required Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Required Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Required Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Block</t>
+  </si>
+  <si>
     <t xml:space="preserve">UPDATED CATEGORY</t>
   </si>
   <si>
+    <t xml:space="preserve">NUTRITION</t>
+  </si>
+  <si>
     <t xml:space="preserve">GRAIN</t>
   </si>
   <si>
+    <t xml:space="preserve">left, right, top, bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxadjc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATED SUBCATEGORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN KID, GRAIN ALL FAMILY, GRAIN ADULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxadjc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelf length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOASTER PASTRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRUIT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN,NUTRITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN, NUTRITION, FRUIT, TOASTER PASTRIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could not determine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxblock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxblockC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANNIE'S HOMEGROWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN KID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxblockC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTRN WELLNESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlkPercent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTRN PERFORMANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTRN DIET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN ALL FAMILY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlkOrientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN ADULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRUIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Present in Grain MSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlkOrientation1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATED FRANCHISE/BRAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blk1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMI_SIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Size</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nat/Org for TRAX</t>
   </si>
   <si>
     <t xml:space="preserve">NATURAL/ORGANIC</t>
   </si>
   <si>
-    <t xml:space="preserve">PrimaryLocation1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRUIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Required Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Required Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B Required Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B Required Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Threshold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUTRITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">left, right, top, bottom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxadjc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B Value 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Required Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B Required Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxadjc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shelf length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOASTER PASTRIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRUIT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN,NUTRITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN, NUTRITION, FRUIT, TOASTER PASTRIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Could not determine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxblock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDATED SUBCATEGORY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxblockC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerator Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerator Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator Param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANNIE'S HOMEGROWN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN KID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxblockC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTRN WELLNESS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BlkPercent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTRN PERFORMANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTRN DIET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN ALL FAMILY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BlkOrientation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN ADULT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAIN KIDS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Present in Grain MSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BlkOrientation1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDATED FRANCHISE/BRAND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIVATE LABEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blk1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMI_SIZE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GRAIN KID, GRAIN ALL FAMILY, GRAIN ADULT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left, Right </t>
+    <t xml:space="preserve">Vector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Other Configuration (Vertical Flow or No Flow)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nat/Org Grain Bars in Grain MSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nat/Org Grain Bars stocked in Nat/Org Aisle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stocked_location_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nat/Org Fruit Snacks in Fruit MSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nat/Org Fruit Snacks stocked in Nat/Org Aisle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stocked_location_2</t>
   </si>
   <si>
     <t xml:space="preserve">Result Key</t>
@@ -540,61 +565,61 @@
     <t xml:space="preserve">Nutrition in the RTE Cereal Aisle, Nutrition in Pharmacy/Health Aisle, Nutrition in Natural/Organic Aisle, Nutrition in Other Aisle / Perimeter</t>
   </si>
   <si>
+    <t xml:space="preserve">Anchor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grain, Nutrition, Fruit, Toaster Pastries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShelfLength </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LESS THAN OR EQUAL TO 4 FT,4 FT &gt; AND &lt;= 8 FT,8 FT &gt; AND &lt;= 12 FT,12 FT &gt; AND &lt;= 16 FT,16 FT &gt; AND &lt;= 20 FT,20 FT &gt; AND &lt;= 24 FT,24 FT &gt; AND &lt;= 28 FT,28 FT &gt; AND &lt;= 32 FT,GREATER THAN 32 FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated Bars Set Present, Non-Integrated Bars Set Present, Could not determine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult,All Family,Kid,Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrition, Toaster Pastries, Fruit; Nutrition, Fruit; Nutrition, Toaster Pastries; Toaster Pastries, Fruit; Nutrition; Fruit; Toaster Pastries; Only Grain; Could not determine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance, Wellness, Diet; Performance, Wellness; Performance, Diet;  Wellness, Diet; Performance; Wellness; Diet; Could not determine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stocked with Kids Grain, Not Stocked with Kids Grain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical,Not Vertical,Not Blocked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical,Not Vertical,Not Blocked,Not Present in Grain MSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blocked, Not Blocked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blocked, Not Blocked, Not Present in Grain MSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult, All Family, Kid; Adult, Kid, All Family; All Family, Adult, Kid; All Family, Kid, Adult; Kid, Adult, All Family; Kid, All Family, Adult; All Other Configuration (Vertical Flow or No Flow)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical, Not Vertical, Not Blocked</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nat/Org Grain Bars in Grain MSL, Nat/Org Grain Bars stocked in Nat/Org Aisle</t>
   </si>
   <si>
-    <t xml:space="preserve">Anchor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grain, Nutrition, Fruit, TP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShelfLength </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LESS THAN OR EQUAL TO 4 FT,4 FT &gt; AND &lt;= 8 FT,8 FT &gt; AND &lt;= 12 FT,12 FT &gt; AND &lt;= 16 FT,16 FT &gt; AND &lt;= 20 FT,20 FT &gt; AND &lt;= 24 FT,24 FT &gt; AND &lt;= 28 FT,28 FT &gt; AND &lt;= 32 FT,GREATER THAN 32 FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrated Bars Set Present, Non-Integrated Bars Set Present, Could not determine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adult,All Family,Kid, Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutrition, Toaster Pastries, Fruit; Nutrition, Fruit; Nutrition, Toaster Pastries; Toaster Pastries, Fruit; Nutrition; Fruit; Toaster Pastries; Only Grain; Could not determine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance, Wellness, Diet; Performance, Wellness; Performance, Diet;  Wellness, Diet; Performance; Wellness; Diet; Could not determine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stocked with Kids Grain, Not Stocked with Kids Grain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertical,Not Vertical,Not Blocked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertical,Not Vertical,Not Blocked,Not Present in Grain MSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blocked, Not Blocked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blocked, Not Blocked, Not Present in Grain MSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psequence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adult, All Family, Kid; Adult, Kid, All Family; All Family, Adult, Kid; All Family, Kid, Adult; Kid, Adult, All Family; Kid, All Family, Adult; All Other Configuration (Vertical Flow or No Flow)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertical, Not Vertical, Not Blocked</t>
+    <t xml:space="preserve">Nat/Org Fruit Snacks in Fruit MSL, Nat/Org Fruit Snacks stocked in Nat/Org Aisle</t>
   </si>
 </sst>
 </file>
@@ -604,13 +629,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -628,16 +652,9 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -645,26 +662,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -728,7 +737,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -753,7 +762,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -761,23 +770,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -785,20 +794,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -812,6 +825,11 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF9DC3E6"/>
@@ -820,6 +838,8 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <family val="2"/>
         <color rgb="FF7F7F7F"/>
       </font>
       <fill>
@@ -829,6 +849,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF70AD47"/>
@@ -836,6 +861,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
@@ -843,6 +873,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC5E0B4"/>
@@ -850,6 +885,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -926,13 +966,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -943,9 +983,9 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.1619433198381"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,591 +1016,611 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="20" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="20" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="41.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="41.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="41.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="20.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J23" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="17" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J24" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H25" s="3"/>
       <c r="I25" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -1572,14 +1632,15 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1588,23 +1649,26 @@
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1613,70 +1677,75 @@
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J29" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1685,202 +1754,204 @@
         <v>53</v>
       </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H33" s="3"/>
       <c r="I33" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J33" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J34" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H35" s="3"/>
       <c r="I35" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J35" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H36" s="3"/>
       <c r="I36" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J36" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G37" s="3"/>
-      <c r="H37" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H37" s="3"/>
       <c r="I37" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H38" s="3"/>
       <c r="I38" s="3" t="s">
-        <v>74</v>
+        <v>12</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H39" s="3"/>
       <c r="I39" s="3" t="s">
-        <v>74</v>
+        <v>12</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I39">
-    <filterColumn colId="1">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Anchor"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J39"/>
   <conditionalFormatting sqref="C28">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>KPIs!$V28="Ready"</formula>
+      <formula>KPIs!$W28="Ready"</formula>
     </cfRule>
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>KPIs!$V28="Removed"</formula>
+      <formula>KPIs!$W28="Removed"</formula>
     </cfRule>
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>KPIs!$V28="Done"</formula>
+      <formula>KPIs!$W28="Done"</formula>
     </cfRule>
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>KPIs!$V28="Built"</formula>
+      <formula>KPIs!$W28="Built"</formula>
     </cfRule>
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>KPIs!$V28="Templated"</formula>
+      <formula>KPIs!$W28="Templated"</formula>
     </cfRule>
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>KPIs!$V28&lt;&gt;""</formula>
+      <formula>KPIs!$W28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1919,43 +1990,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1982,8 +2053,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2002,80 +2073,80 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2083,20 +2154,20 @@
         <v>54</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2115,33 +2186,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.4493927125506"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7449392712551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>82</v>
+        <v>108</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2149,13 +2226,19 @@
         <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2174,10 +2257,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.7975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5222672064777"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="0" width="16.0121457489879"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2189,156 +2389,156 @@
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" s="15" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>162</v>
+        <v>174</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>162</v>
+        <v>177</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>178</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>171</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>173</v>
+        <v>123</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,113 +2546,128 @@
         <v>131</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>177</v>
+        <v>137</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B14" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>171</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>179</v>
+        <v>144</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>180</v>
+        <v>147</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>174</v>
+        <v>190</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2469,10 +2684,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2480,11 +2695,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.0890688259109"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,158 +2705,116 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>97</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2663,8 +2834,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2687,81 +2858,81 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>0.25</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2780,81 +2951,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J65536"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.4858299595142"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9757085020243"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.2267206477733"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8663967611336"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>104</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2874,7 +3045,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2893,30 +3064,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>4</v>
@@ -2925,18 +3096,18 @@
         <v>32</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>120</v>
+        <v>103</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>4</v>
@@ -2945,18 +3116,18 @@
         <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>4</v>
@@ -2965,18 +3136,18 @@
         <v>32</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>4</v>
@@ -2985,18 +3156,18 @@
         <v>32</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>4</v>
@@ -3005,18 +3176,18 @@
         <v>32</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>4</v>
@@ -3025,18 +3196,18 @@
         <v>32</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>4</v>
@@ -3045,18 +3216,18 @@
         <v>32</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>4</v>
@@ -3065,7 +3236,7 @@
         <v>32</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3086,8 +3257,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3100,55 +3271,55 @@
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+    <row r="1" s="12" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>82</v>
+      <c r="C1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="63.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3187,59 +3358,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>128</v>
+        <v>109</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3280,19 +3451,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3300,19 +3471,19 @@
         <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3334,7 +3505,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3351,153 +3522,153 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>147</v>
+        <v>139</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>